<commit_message>
Multiple browser code commit
</commit_message>
<xml_diff>
--- a/TestData/contact_Form_Test.xlsx
+++ b/TestData/contact_Form_Test.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="all_test_data" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="service_test" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="algo_contact" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Sheet4" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Sheet5" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1966" uniqueCount="409">
   <si>
     <t xml:space="preserve">use_case</t>
   </si>
@@ -1488,85 +1489,79 @@
     <t xml:space="preserve">scroll</t>
   </si>
   <si>
+    <t xml:space="preserve">TC_H_01_Header_Contact_Us : All_Fields_Valid (All Required Fields are Valid)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xpath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//*[@id="menu-item-23882"]/a/span</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_H_02_Footer_Contact_Us : All_Fields_Valid (All Required Fields are Valid)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//*[@class='btn contact_us']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//*[text()='Algoworks Solutions Inc.']</t>
+  </si>
+  <si>
     <t xml:space="preserve">TC_H_03_Middle_Contact_Us : All_Fields_Valid (All Required Fields are Valid)</t>
   </si>
   <si>
-    <t xml:space="preserve">xpath</t>
-  </si>
-  <si>
     <t xml:space="preserve">//*[@id="layerslider_15"]/div[1]/div/div[7]/a</t>
   </si>
   <si>
-    <t xml:space="preserve">TC_H_01_Header_Contact_Us : All_Fields_Valid (All Required Fields are Valid)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">//*[@id="menu-item-23882"]/a/span</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thank You – Algoworks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_H_02_Footer_Contact_Us : All_Fields_Valid (All Required Fields are Valid)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">//*[@class='btn contact_us']</t>
-  </si>
-  <si>
-    <t xml:space="preserve">//*[text()='Algoworks Solutions Inc.']</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_H_04_Middle_Contact_Us : All_Fields_Null  (All Required Fields are Blank)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_H_05_Middle_Contact_Us : All_Fields_Valid (All Required Fields are Valid)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_H_06_Middle_Contact_Us :Email_Validation ( Email without “@gmail.com” )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_H_07_Middle_Contact_Us :Email_Validation ( Email including “AT” instead of “@” )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_H_08_Middle_Contact_Us :Email_Validation ( Email without “.com” )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_H_09_Middle_Contact_Us :Email_Validation ( Email without “@”) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_H_10_Middle_Contact_Us :Email_Validation ( Email without valid name ) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_H_11_Middle_Contact_Us :Email_Validation ( Blank Email ) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_H_12_Middle_Contact_Us :Email_Validation ( Email without dot symbol )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_H_13_Middle_Contact_Us :Phone_Validation( Phone including alphabet &amp; special Char)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_H_14_Middle_Contact_Us :Phone_Validation ( Blank Phone)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_H_15_Middle_Contact_Us :Phone_Validation ( Phone including less than 10 digits)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_H_16_Middle_Contact_Us :Phone_Validation ( Phone including more than 10 digits)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_H_17_Middle_Contact_Us :Name_Validation (Name including Numbers)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_H_18_Middle_Contact_Us :Name_Validation (Name including Alphanumeric)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_H_19_Middle_Contact_Us :Name_Validation (Name including special character)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_H_20_Middle_Contact_Us :Name_Validation (Blank Name)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_H_21_Middle_Contact_Us :Message_Validation (Blank Message)</t>
+    <t xml:space="preserve">TC_H_04_Header_Contact_Us : All_Fields_Null  (All Required Fields are Blank)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_H_06_Header_Contact_Us :Email_Validation ( Email without “@gmail.com” )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_H_07_Header_Contact_Us :Email_Validation ( Email including “AT” instead of “@” )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_H_08_Header_Contact_Us :Email_Validation ( Email without “.com” )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_H_09_Header_Contact_Us :Email_Validation ( Email without “@”) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_H_10_Header_Contact_Us :Email_Validation ( Email without valid name ) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_H_11_Header_Contact_Us :Email_Validation ( Blank Email ) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_H_12_Header_Contact_Us :Email_Validation ( Email without dot symbol )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_H_13_Header_Contact_Us :Phone_Validation( Phone including alphabet &amp; special Char)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_H_14_Header_Contact_Us :Phone_Validation ( Blank Phone)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_H_15_Header_Contact_Us :Phone_Validation ( Phone including less than 10 digits)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_H_16_Header_Contact_Us :Phone_Validation ( Phone including more than 10 digits)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_H_17_Header_Contact_Us :Name_Validation (Name including Numbers)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_H_18_Header_Contact_Us :Name_Validation (Name including Alphanumeric)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_H_19_Header_Contact_Us :Name_Validation (Name including special character)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_H_20_Header_Contact_Us :Name_Validation (Blank Name)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_H_21_Header_Contact_Us :Message_Validation (Blank Message)</t>
   </si>
 </sst>
 </file>
@@ -1816,7 +1811,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A25" activeCellId="1" sqref="2:2 A25"/>
+      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2218,8 +2213,8 @@
   </sheetPr>
   <dimension ref="A1:AMH136"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A121" activeCellId="1" sqref="2:2 A121"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5434,10 +5429,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="2:2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5497,9 +5492,6 @@
       <c r="C2" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>47</v>
-      </c>
       <c r="F2" s="0" t="s">
         <v>9</v>
       </c>
@@ -5514,11 +5506,500 @@
       </c>
       <c r="J2" s="1" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>387</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>9805674556</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>390</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>9805674556</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>9805674556</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>9805674556</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>9805674556</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>9805674556</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>9805674556</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>9805674556</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>9805674556</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="4" t="n">
+        <v>98675645</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="4" t="n">
+        <v>986756459876543</v>
+      </c>
+      <c r="I16" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>563653673673</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>9805674556</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>9805674556</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <v>9805674556</v>
+      </c>
+      <c r="I19" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>9805674556</v>
+      </c>
+      <c r="I20" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>9805674556</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" display="mamta.mehta@algoworks.com"/>
+    <hyperlink ref="G3" r:id="rId2" display="mamta.mehta@algoworks.com"/>
+    <hyperlink ref="G4" r:id="rId3" display="mamta.mehta@algoworks.com"/>
+    <hyperlink ref="G8" r:id="rId4" display="mamtamehta@gmail"/>
+    <hyperlink ref="G12" r:id="rId5" display="mamtamehta@gmailcom"/>
+    <hyperlink ref="G13" r:id="rId6" display="mamta.mehta@algoworks.com"/>
+    <hyperlink ref="G14" r:id="rId7" display="mamta.mehta@algoworks.com"/>
+    <hyperlink ref="G15" r:id="rId8" display="mamta.mehta@algoworks.com"/>
+    <hyperlink ref="G16" r:id="rId9" display="mamta.mehta@algoworks.com"/>
+    <hyperlink ref="G17" r:id="rId10" display="mamta.mehta@algoworks.com"/>
+    <hyperlink ref="G18" r:id="rId11" display="mamta.mehta@algoworks.com"/>
+    <hyperlink ref="G19" r:id="rId12" display="mamta.mehta@algoworks.com"/>
+    <hyperlink ref="G20" r:id="rId13" display="mamta.mehta@algoworks.com"/>
+    <hyperlink ref="G21" r:id="rId14" display="mamta.mehta@algoworks.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -5535,10 +6016,3228 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:AMH136"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="2:2 A4"/>
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="51.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="70.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.77"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="G45" s="3"/>
+      <c r="H45" s="1"/>
+      <c r="K45" s="1"/>
+      <c r="M45" s="3"/>
+      <c r="N45" s="1"/>
+      <c r="Q45" s="1"/>
+      <c r="S45" s="3"/>
+      <c r="T45" s="1"/>
+      <c r="W45" s="1"/>
+      <c r="Y45" s="3"/>
+      <c r="Z45" s="1"/>
+      <c r="AC45" s="1"/>
+      <c r="AE45" s="3"/>
+      <c r="AF45" s="1"/>
+      <c r="AI45" s="1"/>
+      <c r="AK45" s="3"/>
+      <c r="AL45" s="1"/>
+      <c r="AO45" s="1"/>
+      <c r="AQ45" s="3"/>
+      <c r="AR45" s="1"/>
+      <c r="AU45" s="1"/>
+      <c r="AW45" s="3"/>
+      <c r="AX45" s="1"/>
+      <c r="BA45" s="1"/>
+      <c r="BC45" s="3"/>
+      <c r="BD45" s="1"/>
+      <c r="BG45" s="1"/>
+      <c r="BI45" s="3"/>
+      <c r="BJ45" s="1"/>
+      <c r="BM45" s="1"/>
+      <c r="BO45" s="3"/>
+      <c r="BP45" s="1"/>
+      <c r="BS45" s="1"/>
+      <c r="BU45" s="3"/>
+      <c r="BV45" s="1"/>
+      <c r="BY45" s="1"/>
+      <c r="CA45" s="3"/>
+      <c r="CB45" s="1"/>
+      <c r="CE45" s="1"/>
+      <c r="CG45" s="3"/>
+      <c r="CH45" s="1"/>
+      <c r="CK45" s="1"/>
+      <c r="CM45" s="3"/>
+      <c r="CN45" s="1"/>
+      <c r="CQ45" s="1"/>
+      <c r="CS45" s="3"/>
+      <c r="CT45" s="1"/>
+      <c r="CW45" s="1"/>
+      <c r="CY45" s="3"/>
+      <c r="CZ45" s="1"/>
+      <c r="DC45" s="1"/>
+      <c r="DE45" s="3"/>
+      <c r="DF45" s="1"/>
+      <c r="DI45" s="1"/>
+      <c r="DK45" s="3"/>
+      <c r="DL45" s="1"/>
+      <c r="DO45" s="1"/>
+      <c r="DQ45" s="3"/>
+      <c r="DR45" s="1"/>
+      <c r="DU45" s="1"/>
+      <c r="DW45" s="3"/>
+      <c r="DX45" s="1"/>
+      <c r="EA45" s="1"/>
+      <c r="EC45" s="3"/>
+      <c r="ED45" s="1"/>
+      <c r="EG45" s="1"/>
+      <c r="EI45" s="3"/>
+      <c r="EJ45" s="1"/>
+      <c r="EM45" s="1"/>
+      <c r="EO45" s="3"/>
+      <c r="EP45" s="1"/>
+      <c r="ES45" s="1"/>
+      <c r="EU45" s="3"/>
+      <c r="EV45" s="1"/>
+      <c r="EY45" s="1"/>
+      <c r="FA45" s="3"/>
+      <c r="FB45" s="1"/>
+      <c r="FE45" s="1"/>
+      <c r="FG45" s="3"/>
+      <c r="FH45" s="1"/>
+      <c r="FK45" s="1"/>
+      <c r="FM45" s="3"/>
+      <c r="FN45" s="1"/>
+      <c r="FQ45" s="1"/>
+      <c r="FS45" s="3"/>
+      <c r="FT45" s="1"/>
+      <c r="FW45" s="1"/>
+      <c r="FY45" s="3"/>
+      <c r="FZ45" s="1"/>
+      <c r="GC45" s="1"/>
+      <c r="GE45" s="3"/>
+      <c r="GF45" s="1"/>
+      <c r="GI45" s="1"/>
+      <c r="GK45" s="3"/>
+      <c r="GL45" s="1"/>
+      <c r="GO45" s="1"/>
+      <c r="GQ45" s="3"/>
+      <c r="GR45" s="1"/>
+      <c r="GU45" s="1"/>
+      <c r="GW45" s="3"/>
+      <c r="GX45" s="1"/>
+      <c r="HA45" s="1"/>
+      <c r="HC45" s="3"/>
+      <c r="HD45" s="1"/>
+      <c r="HG45" s="1"/>
+      <c r="HI45" s="3"/>
+      <c r="HJ45" s="1"/>
+      <c r="HM45" s="1"/>
+      <c r="HO45" s="3"/>
+      <c r="HP45" s="1"/>
+      <c r="HS45" s="1"/>
+      <c r="HU45" s="3"/>
+      <c r="HV45" s="1"/>
+      <c r="HY45" s="1"/>
+      <c r="IA45" s="3"/>
+      <c r="IB45" s="1"/>
+      <c r="IE45" s="1"/>
+      <c r="IG45" s="3"/>
+      <c r="IH45" s="1"/>
+      <c r="IK45" s="1"/>
+      <c r="IM45" s="3"/>
+      <c r="IN45" s="1"/>
+      <c r="IQ45" s="1"/>
+      <c r="IS45" s="3"/>
+      <c r="IT45" s="1"/>
+      <c r="IW45" s="1"/>
+      <c r="IY45" s="3"/>
+      <c r="IZ45" s="1"/>
+      <c r="JC45" s="1"/>
+      <c r="JE45" s="3"/>
+      <c r="JF45" s="1"/>
+      <c r="JI45" s="1"/>
+      <c r="JK45" s="3"/>
+      <c r="JL45" s="1"/>
+      <c r="JO45" s="1"/>
+      <c r="JQ45" s="3"/>
+      <c r="JR45" s="1"/>
+      <c r="JU45" s="1"/>
+      <c r="JW45" s="3"/>
+      <c r="JX45" s="1"/>
+      <c r="KA45" s="1"/>
+      <c r="KC45" s="3"/>
+      <c r="KD45" s="1"/>
+      <c r="KG45" s="1"/>
+      <c r="KI45" s="3"/>
+      <c r="KJ45" s="1"/>
+      <c r="KM45" s="1"/>
+      <c r="KO45" s="3"/>
+      <c r="KP45" s="1"/>
+      <c r="KS45" s="1"/>
+      <c r="KU45" s="3"/>
+      <c r="KV45" s="1"/>
+      <c r="KY45" s="1"/>
+      <c r="LA45" s="3"/>
+      <c r="LB45" s="1"/>
+      <c r="LE45" s="1"/>
+      <c r="LG45" s="3"/>
+      <c r="LH45" s="1"/>
+      <c r="LK45" s="1"/>
+      <c r="LM45" s="3"/>
+      <c r="LN45" s="1"/>
+      <c r="LQ45" s="1"/>
+      <c r="LS45" s="3"/>
+      <c r="LT45" s="1"/>
+      <c r="LW45" s="1"/>
+      <c r="LY45" s="3"/>
+      <c r="LZ45" s="1"/>
+      <c r="MC45" s="1"/>
+      <c r="ME45" s="3"/>
+      <c r="MF45" s="1"/>
+      <c r="MI45" s="1"/>
+      <c r="MK45" s="3"/>
+      <c r="ML45" s="1"/>
+      <c r="MO45" s="1"/>
+      <c r="MQ45" s="3"/>
+      <c r="MR45" s="1"/>
+      <c r="MU45" s="1"/>
+      <c r="MW45" s="3"/>
+      <c r="MX45" s="1"/>
+      <c r="NA45" s="1"/>
+      <c r="NC45" s="3"/>
+      <c r="ND45" s="1"/>
+      <c r="NG45" s="1"/>
+      <c r="NI45" s="3"/>
+      <c r="NJ45" s="1"/>
+      <c r="NM45" s="1"/>
+      <c r="NO45" s="3"/>
+      <c r="NP45" s="1"/>
+      <c r="NS45" s="1"/>
+      <c r="NU45" s="3"/>
+      <c r="NV45" s="1"/>
+      <c r="NY45" s="1"/>
+      <c r="OA45" s="3"/>
+      <c r="OB45" s="1"/>
+      <c r="OE45" s="1"/>
+      <c r="OG45" s="3"/>
+      <c r="OH45" s="1"/>
+      <c r="OK45" s="1"/>
+      <c r="OM45" s="3"/>
+      <c r="ON45" s="1"/>
+      <c r="OQ45" s="1"/>
+      <c r="OS45" s="3"/>
+      <c r="OT45" s="1"/>
+      <c r="OW45" s="1"/>
+      <c r="OY45" s="3"/>
+      <c r="OZ45" s="1"/>
+      <c r="PC45" s="1"/>
+      <c r="PE45" s="3"/>
+      <c r="PF45" s="1"/>
+      <c r="PI45" s="1"/>
+      <c r="PK45" s="3"/>
+      <c r="PL45" s="1"/>
+      <c r="PO45" s="1"/>
+      <c r="PQ45" s="3"/>
+      <c r="PR45" s="1"/>
+      <c r="PU45" s="1"/>
+      <c r="PW45" s="3"/>
+      <c r="PX45" s="1"/>
+      <c r="QA45" s="1"/>
+      <c r="QC45" s="3"/>
+      <c r="QD45" s="1"/>
+      <c r="QG45" s="1"/>
+      <c r="QI45" s="3"/>
+      <c r="QJ45" s="1"/>
+      <c r="QM45" s="1"/>
+      <c r="QO45" s="3"/>
+      <c r="QP45" s="1"/>
+      <c r="QS45" s="1"/>
+      <c r="QU45" s="3"/>
+      <c r="QV45" s="1"/>
+      <c r="QY45" s="1"/>
+      <c r="RA45" s="3"/>
+      <c r="RB45" s="1"/>
+      <c r="RE45" s="1"/>
+      <c r="RG45" s="3"/>
+      <c r="RH45" s="1"/>
+      <c r="RK45" s="1"/>
+      <c r="RM45" s="3"/>
+      <c r="RN45" s="1"/>
+      <c r="RQ45" s="1"/>
+      <c r="RS45" s="3"/>
+      <c r="RT45" s="1"/>
+      <c r="RW45" s="1"/>
+      <c r="RY45" s="3"/>
+      <c r="RZ45" s="1"/>
+      <c r="SC45" s="1"/>
+      <c r="SE45" s="3"/>
+      <c r="SF45" s="1"/>
+      <c r="SI45" s="1"/>
+      <c r="SK45" s="3"/>
+      <c r="SL45" s="1"/>
+      <c r="SO45" s="1"/>
+      <c r="SQ45" s="3"/>
+      <c r="SR45" s="1"/>
+      <c r="SU45" s="1"/>
+      <c r="SW45" s="3"/>
+      <c r="SX45" s="1"/>
+      <c r="TA45" s="1"/>
+      <c r="TC45" s="3"/>
+      <c r="TD45" s="1"/>
+      <c r="TG45" s="1"/>
+      <c r="TI45" s="3"/>
+      <c r="TJ45" s="1"/>
+      <c r="TM45" s="1"/>
+      <c r="TO45" s="3"/>
+      <c r="TP45" s="1"/>
+      <c r="TS45" s="1"/>
+      <c r="TU45" s="3"/>
+      <c r="TV45" s="1"/>
+      <c r="TY45" s="1"/>
+      <c r="UA45" s="3"/>
+      <c r="UB45" s="1"/>
+      <c r="UE45" s="1"/>
+      <c r="UG45" s="3"/>
+      <c r="UH45" s="1"/>
+      <c r="UK45" s="1"/>
+      <c r="UM45" s="3"/>
+      <c r="UN45" s="1"/>
+      <c r="UQ45" s="1"/>
+      <c r="US45" s="3"/>
+      <c r="UT45" s="1"/>
+      <c r="UW45" s="1"/>
+      <c r="UY45" s="3"/>
+      <c r="UZ45" s="1"/>
+      <c r="VC45" s="1"/>
+      <c r="VE45" s="3"/>
+      <c r="VF45" s="1"/>
+      <c r="VI45" s="1"/>
+      <c r="VK45" s="3"/>
+      <c r="VL45" s="1"/>
+      <c r="VO45" s="1"/>
+      <c r="VQ45" s="3"/>
+      <c r="VR45" s="1"/>
+      <c r="VU45" s="1"/>
+      <c r="VW45" s="3"/>
+      <c r="VX45" s="1"/>
+      <c r="WA45" s="1"/>
+      <c r="WC45" s="3"/>
+      <c r="WD45" s="1"/>
+      <c r="WG45" s="1"/>
+      <c r="WI45" s="3"/>
+      <c r="WJ45" s="1"/>
+      <c r="WM45" s="1"/>
+      <c r="WO45" s="3"/>
+      <c r="WP45" s="1"/>
+      <c r="WS45" s="1"/>
+      <c r="WU45" s="3"/>
+      <c r="WV45" s="1"/>
+      <c r="WY45" s="1"/>
+      <c r="XA45" s="3"/>
+      <c r="XB45" s="1"/>
+      <c r="XE45" s="1"/>
+      <c r="XG45" s="3"/>
+      <c r="XH45" s="1"/>
+      <c r="XK45" s="1"/>
+      <c r="XM45" s="3"/>
+      <c r="XN45" s="1"/>
+      <c r="XQ45" s="1"/>
+      <c r="XS45" s="3"/>
+      <c r="XT45" s="1"/>
+      <c r="XW45" s="1"/>
+      <c r="XY45" s="3"/>
+      <c r="XZ45" s="1"/>
+      <c r="YC45" s="1"/>
+      <c r="YE45" s="3"/>
+      <c r="YF45" s="1"/>
+      <c r="YI45" s="1"/>
+      <c r="YK45" s="3"/>
+      <c r="YL45" s="1"/>
+      <c r="YO45" s="1"/>
+      <c r="YQ45" s="3"/>
+      <c r="YR45" s="1"/>
+      <c r="YU45" s="1"/>
+      <c r="YW45" s="3"/>
+      <c r="YX45" s="1"/>
+      <c r="ZA45" s="1"/>
+      <c r="ZC45" s="3"/>
+      <c r="ZD45" s="1"/>
+      <c r="ZG45" s="1"/>
+      <c r="ZI45" s="3"/>
+      <c r="ZJ45" s="1"/>
+      <c r="ZM45" s="1"/>
+      <c r="ZO45" s="3"/>
+      <c r="ZP45" s="1"/>
+      <c r="ZS45" s="1"/>
+      <c r="ZU45" s="3"/>
+      <c r="ZV45" s="1"/>
+      <c r="ZY45" s="1"/>
+      <c r="AAA45" s="3"/>
+      <c r="AAB45" s="1"/>
+      <c r="AAE45" s="1"/>
+      <c r="AAG45" s="3"/>
+      <c r="AAH45" s="1"/>
+      <c r="AAK45" s="1"/>
+      <c r="AAM45" s="3"/>
+      <c r="AAN45" s="1"/>
+      <c r="AAQ45" s="1"/>
+      <c r="AAS45" s="3"/>
+      <c r="AAT45" s="1"/>
+      <c r="AAW45" s="1"/>
+      <c r="AAY45" s="3"/>
+      <c r="AAZ45" s="1"/>
+      <c r="ABC45" s="1"/>
+      <c r="ABE45" s="3"/>
+      <c r="ABF45" s="1"/>
+      <c r="ABI45" s="1"/>
+      <c r="ABK45" s="3"/>
+      <c r="ABL45" s="1"/>
+      <c r="ABO45" s="1"/>
+      <c r="ABQ45" s="3"/>
+      <c r="ABR45" s="1"/>
+      <c r="ABU45" s="1"/>
+      <c r="ABW45" s="3"/>
+      <c r="ABX45" s="1"/>
+      <c r="ACA45" s="1"/>
+      <c r="ACC45" s="3"/>
+      <c r="ACD45" s="1"/>
+      <c r="ACG45" s="1"/>
+      <c r="ACI45" s="3"/>
+      <c r="ACJ45" s="1"/>
+      <c r="ACM45" s="1"/>
+      <c r="ACO45" s="3"/>
+      <c r="ACP45" s="1"/>
+      <c r="ACS45" s="1"/>
+      <c r="ACU45" s="3"/>
+      <c r="ACV45" s="1"/>
+      <c r="ACY45" s="1"/>
+      <c r="ADA45" s="3"/>
+      <c r="ADB45" s="1"/>
+      <c r="ADE45" s="1"/>
+      <c r="ADG45" s="3"/>
+      <c r="ADH45" s="1"/>
+      <c r="ADK45" s="1"/>
+      <c r="ADM45" s="3"/>
+      <c r="ADN45" s="1"/>
+      <c r="ADQ45" s="1"/>
+      <c r="ADS45" s="3"/>
+      <c r="ADT45" s="1"/>
+      <c r="ADW45" s="1"/>
+      <c r="ADY45" s="3"/>
+      <c r="ADZ45" s="1"/>
+      <c r="AEC45" s="1"/>
+      <c r="AEE45" s="3"/>
+      <c r="AEF45" s="1"/>
+      <c r="AEI45" s="1"/>
+      <c r="AEK45" s="3"/>
+      <c r="AEL45" s="1"/>
+      <c r="AEO45" s="1"/>
+      <c r="AEQ45" s="3"/>
+      <c r="AER45" s="1"/>
+      <c r="AEU45" s="1"/>
+      <c r="AEW45" s="3"/>
+      <c r="AEX45" s="1"/>
+      <c r="AFA45" s="1"/>
+      <c r="AFC45" s="3"/>
+      <c r="AFD45" s="1"/>
+      <c r="AFG45" s="1"/>
+      <c r="AFI45" s="3"/>
+      <c r="AFJ45" s="1"/>
+      <c r="AFM45" s="1"/>
+      <c r="AFO45" s="3"/>
+      <c r="AFP45" s="1"/>
+      <c r="AFS45" s="1"/>
+      <c r="AFU45" s="3"/>
+      <c r="AFV45" s="1"/>
+      <c r="AFY45" s="1"/>
+      <c r="AGA45" s="3"/>
+      <c r="AGB45" s="1"/>
+      <c r="AGE45" s="1"/>
+      <c r="AGG45" s="3"/>
+      <c r="AGH45" s="1"/>
+      <c r="AGK45" s="1"/>
+      <c r="AGM45" s="3"/>
+      <c r="AGN45" s="1"/>
+      <c r="AGQ45" s="1"/>
+      <c r="AGS45" s="3"/>
+      <c r="AGT45" s="1"/>
+      <c r="AGW45" s="1"/>
+      <c r="AGY45" s="3"/>
+      <c r="AGZ45" s="1"/>
+      <c r="AHC45" s="1"/>
+      <c r="AHE45" s="3"/>
+      <c r="AHF45" s="1"/>
+      <c r="AHI45" s="1"/>
+      <c r="AHK45" s="3"/>
+      <c r="AHL45" s="1"/>
+      <c r="AHO45" s="1"/>
+      <c r="AHQ45" s="3"/>
+      <c r="AHR45" s="1"/>
+      <c r="AHU45" s="1"/>
+      <c r="AHW45" s="3"/>
+      <c r="AHX45" s="1"/>
+      <c r="AIA45" s="1"/>
+      <c r="AIC45" s="3"/>
+      <c r="AID45" s="1"/>
+      <c r="AIG45" s="1"/>
+      <c r="AII45" s="3"/>
+      <c r="AIJ45" s="1"/>
+      <c r="AIM45" s="1"/>
+      <c r="AIO45" s="3"/>
+      <c r="AIP45" s="1"/>
+      <c r="AIS45" s="1"/>
+      <c r="AIU45" s="3"/>
+      <c r="AIV45" s="1"/>
+      <c r="AIY45" s="1"/>
+      <c r="AJA45" s="3"/>
+      <c r="AJB45" s="1"/>
+      <c r="AJE45" s="1"/>
+      <c r="AJG45" s="3"/>
+      <c r="AJH45" s="1"/>
+      <c r="AJK45" s="1"/>
+      <c r="AJM45" s="3"/>
+      <c r="AJN45" s="1"/>
+      <c r="AJQ45" s="1"/>
+      <c r="AJS45" s="3"/>
+      <c r="AJT45" s="1"/>
+      <c r="AJW45" s="1"/>
+      <c r="AJY45" s="3"/>
+      <c r="AJZ45" s="1"/>
+      <c r="AKC45" s="1"/>
+      <c r="AKE45" s="3"/>
+      <c r="AKF45" s="1"/>
+      <c r="AKI45" s="1"/>
+      <c r="AKK45" s="3"/>
+      <c r="AKL45" s="1"/>
+      <c r="AKO45" s="1"/>
+      <c r="AKQ45" s="3"/>
+      <c r="AKR45" s="1"/>
+      <c r="AKU45" s="1"/>
+      <c r="AKW45" s="3"/>
+      <c r="AKX45" s="1"/>
+      <c r="ALA45" s="1"/>
+      <c r="ALC45" s="3"/>
+      <c r="ALD45" s="1"/>
+      <c r="ALG45" s="1"/>
+      <c r="ALI45" s="3"/>
+      <c r="ALJ45" s="1"/>
+      <c r="ALM45" s="1"/>
+      <c r="ALO45" s="3"/>
+      <c r="ALP45" s="1"/>
+      <c r="ALS45" s="1"/>
+      <c r="ALU45" s="3"/>
+      <c r="ALV45" s="1"/>
+      <c r="ALY45" s="1"/>
+      <c r="AMA45" s="3"/>
+      <c r="AMB45" s="1"/>
+      <c r="AME45" s="1"/>
+      <c r="AMG45" s="3"/>
+      <c r="AMH45" s="1"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <v>1700</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <v>2400</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F47" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>3100</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F48" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>3800</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F49" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>4500</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F50" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>5200</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C52" s="0" t="n">
+        <v>5900</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F52" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F53" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F54" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F55" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F56" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F57" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F58" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F59" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F60" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="D61" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F61" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="D62" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F62" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F63" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="D64" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F64" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="D65" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F65" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="D66" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F66" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="D67" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F67" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="D68" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F68" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="D69" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F69" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="D70" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F70" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="C71" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="D71" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F71" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="B72" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="D72" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F72" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="C73" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="D73" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F73" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="C74" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="D74" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F74" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="C75" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="D75" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F75" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="B76" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="C76" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="D76" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F76" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="B77" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="C77" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="D77" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F77" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B78" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="C78" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="D78" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F78" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="B79" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="D79" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F79" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="B80" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="C80" s="0" t="s">
+        <v>250</v>
+      </c>
+      <c r="D80" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F80" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="B81" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="C81" s="0" t="s">
+        <v>253</v>
+      </c>
+      <c r="D81" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F81" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="C82" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="D82" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F82" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="B83" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="C83" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="D83" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F83" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="B84" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="D84" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F84" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="B85" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="C85" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="D85" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F85" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="B86" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="C86" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="D86" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F86" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="B87" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="C87" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="D87" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F87" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="B88" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="C88" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="D88" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F88" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="B89" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="C89" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="D89" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F89" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="B90" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="C90" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="D90" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F90" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="B91" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="C91" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="D91" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F91" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="B92" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="D92" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F92" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="B93" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="C93" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="D93" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F93" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="B94" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="D94" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F94" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="B95" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="C95" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="D95" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F95" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="B96" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="D96" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F96" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="B97" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="C97" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="D97" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F97" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="B98" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="D98" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F98" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="B99" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="C99" s="0" t="s">
+        <v>290</v>
+      </c>
+      <c r="D99" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F99" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="B100" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="D100" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F100" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="B101" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="C101" s="0" t="s">
+        <v>294</v>
+      </c>
+      <c r="D101" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F101" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="102" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="B102" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="D102" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="E102" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F102" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="103" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="B103" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="C103" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="D103" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="E103" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F103" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="104" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="B104" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="D104" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E104" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F104" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="105" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="B105" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="C105" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="D105" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E105" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F105" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="B106" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="C106" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="D106" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E106" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F106" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="B107" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="C107" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="D107" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="E107" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F107" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="B108" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="C108" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="D108" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="E108" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F108" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="B109" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="C109" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="D109" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E109" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F109" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="110" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="B110" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="D110" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="E110" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F110" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="111" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="B111" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="D111" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="E111" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F111" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="112" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="B112" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="C112" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="D112" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E112" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F112" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="113" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="B113" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="C113" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="D113" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="E113" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F113" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="114" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="B114" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="C114" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="D114" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E114" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F114" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="115" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="B115" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="C115" s="0"/>
+      <c r="D115" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="E115" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F115" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="116" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="B116" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="C116" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="D116" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E116" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F116" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="117" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="B117" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="C117" s="0" t="s">
+        <v>321</v>
+      </c>
+      <c r="D117" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="E117" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F117" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="118" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="B118" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="C118" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="D118" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E118" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F118" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="119" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="B119" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="C119" s="0"/>
+      <c r="D119" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E119" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F119" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="120" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="B120" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="C120" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="D120" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="E120" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F120" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="B121" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="C121" s="0" t="s">
+        <v>339</v>
+      </c>
+      <c r="D121" s="0" t="s">
+        <v>340</v>
+      </c>
+      <c r="E121" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F121" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="B122" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="C122" s="0" t="s">
+        <v>342</v>
+      </c>
+      <c r="D122" s="0" t="s">
+        <v>343</v>
+      </c>
+      <c r="E122" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F122" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="B123" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="C123" s="0" t="s">
+        <v>345</v>
+      </c>
+      <c r="D123" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="E123" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F123" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="B124" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="C124" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="D124" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="E124" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F124" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="B125" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="C125" s="0" t="s">
+        <v>351</v>
+      </c>
+      <c r="D125" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E125" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F125" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="126" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="B126" s="6" t="s">
+        <v>353</v>
+      </c>
+      <c r="C126" s="0" t="s">
+        <v>354</v>
+      </c>
+      <c r="D126" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E126" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F126" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="127" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="B127" s="6" t="s">
+        <v>353</v>
+      </c>
+      <c r="C127" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="D127" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E127" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F127" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="128" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="B128" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="C128" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="D128" s="6" t="s">
+        <v>360</v>
+      </c>
+      <c r="E128" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F128" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="129" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="B129" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="C129" s="6" t="s">
+        <v>362</v>
+      </c>
+      <c r="D129" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E129" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F129" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="130" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="B130" s="6" t="s">
+        <v>364</v>
+      </c>
+      <c r="C130" s="0"/>
+      <c r="D130" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E130" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F130" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="131" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="B131" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="C131" s="0"/>
+      <c r="D131" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="E131" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F131" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="132" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="B132" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="C132" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="D132" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E132" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F132" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="133" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="B133" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="C133" s="0"/>
+      <c r="D133" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="E133" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F133" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="134" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="5" t="s">
+        <v>372</v>
+      </c>
+      <c r="B134" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="C134" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="D134" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E134" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F134" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="135" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="B135" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="C135" s="0" t="s">
+        <v>376</v>
+      </c>
+      <c r="D135" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="E135" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F135" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="136" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="B136" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="C136" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="D136" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E136" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F136" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J21"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5590,13 +9289,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>385</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>9</v>
@@ -5611,21 +9310,21 @@
         <v>11</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>389</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>385</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>9</v>
@@ -5645,13 +9344,13 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>384</v>
+        <v>390</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>385</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>386</v>
+        <v>391</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>47</v>
@@ -5674,7 +9373,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>385</v>
@@ -5682,16 +9381,13 @@
       <c r="C5" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="E5" s="0" t="s">
-        <v>47</v>
-      </c>
       <c r="J5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>385</v>
@@ -5699,14 +9395,11 @@
       <c r="C6" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="E6" s="0" t="s">
-        <v>47</v>
-      </c>
       <c r="F6" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>10</v>
+      <c r="G6" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="H6" s="0" t="n">
         <v>9805674556</v>
@@ -5715,12 +9408,12 @@
         <v>11</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>385</v>
@@ -5728,14 +9421,11 @@
       <c r="C7" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="E7" s="0" t="s">
-        <v>47</v>
-      </c>
       <c r="F7" s="0" t="s">
         <v>9</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H7" s="0" t="n">
         <v>9805674556</v>
@@ -5749,7 +9439,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>385</v>
@@ -5757,14 +9447,11 @@
       <c r="C8" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="E8" s="0" t="s">
-        <v>47</v>
-      </c>
       <c r="F8" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="0" t="s">
-        <v>16</v>
+      <c r="G8" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="H8" s="0" t="n">
         <v>9805674556</v>
@@ -5778,7 +9465,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>385</v>
@@ -5786,14 +9473,11 @@
       <c r="C9" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="E9" s="0" t="s">
-        <v>47</v>
-      </c>
       <c r="F9" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>18</v>
+      <c r="G9" s="0" t="s">
+        <v>20</v>
       </c>
       <c r="H9" s="0" t="n">
         <v>9805674556</v>
@@ -5807,7 +9491,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>385</v>
@@ -5815,14 +9499,11 @@
       <c r="C10" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="E10" s="0" t="s">
-        <v>47</v>
-      </c>
       <c r="F10" s="0" t="s">
         <v>9</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H10" s="0" t="n">
         <v>9805674556</v>
@@ -5836,7 +9517,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>385</v>
@@ -5844,15 +9525,9 @@
       <c r="C11" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="E11" s="0" t="s">
-        <v>47</v>
-      </c>
       <c r="F11" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="0" t="s">
-        <v>22</v>
-      </c>
       <c r="H11" s="0" t="n">
         <v>9805674556</v>
       </c>
@@ -5865,7 +9540,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>385</v>
@@ -5873,12 +9548,12 @@
       <c r="C12" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="E12" s="0" t="s">
-        <v>47</v>
-      </c>
       <c r="F12" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="G12" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="H12" s="0" t="n">
         <v>9805674556</v>
       </c>
@@ -5891,7 +9566,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>385</v>
@@ -5899,17 +9574,14 @@
       <c r="C13" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="E13" s="0" t="s">
-        <v>47</v>
-      </c>
       <c r="F13" s="0" t="s">
         <v>9</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H13" s="0" t="n">
-        <v>9805674556</v>
+        <v>10</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="I13" s="0" t="s">
         <v>11</v>
@@ -5920,7 +9592,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>385</v>
@@ -5928,18 +9600,12 @@
       <c r="C14" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="E14" s="0" t="s">
-        <v>47</v>
-      </c>
       <c r="F14" s="0" t="s">
         <v>9</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H14" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="I14" s="0" t="s">
         <v>11</v>
       </c>
@@ -5949,7 +9615,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>385</v>
@@ -5957,15 +9623,15 @@
       <c r="C15" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="E15" s="0" t="s">
-        <v>47</v>
-      </c>
       <c r="F15" s="0" t="s">
         <v>9</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="H15" s="4" t="n">
+        <v>98675645</v>
+      </c>
       <c r="I15" s="0" t="s">
         <v>11</v>
       </c>
@@ -5975,7 +9641,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>385</v>
@@ -5983,9 +9649,6 @@
       <c r="C16" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="E16" s="0" t="s">
-        <v>47</v>
-      </c>
       <c r="F16" s="0" t="s">
         <v>9</v>
       </c>
@@ -5993,7 +9656,7 @@
         <v>10</v>
       </c>
       <c r="H16" s="4" t="n">
-        <v>98675645</v>
+        <v>986756459876543</v>
       </c>
       <c r="I16" s="0" t="s">
         <v>11</v>
@@ -6004,7 +9667,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>385</v>
@@ -6012,17 +9675,14 @@
       <c r="C17" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="E17" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>9</v>
+      <c r="F17" s="0" t="n">
+        <v>563653673673</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H17" s="4" t="n">
-        <v>986756459876543</v>
+      <c r="H17" s="0" t="n">
+        <v>9805674556</v>
       </c>
       <c r="I17" s="0" t="s">
         <v>11</v>
@@ -6033,7 +9693,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>385</v>
@@ -6041,11 +9701,8 @@
       <c r="C18" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="E18" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="F18" s="0" t="n">
-        <v>563653673673</v>
+      <c r="F18" s="0" t="s">
+        <v>33</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>10</v>
@@ -6062,7 +9719,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>385</v>
@@ -6070,11 +9727,8 @@
       <c r="C19" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="E19" s="0" t="s">
-        <v>47</v>
-      </c>
       <c r="F19" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>10</v>
@@ -6091,7 +9745,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>385</v>
@@ -6099,12 +9753,6 @@
       <c r="C20" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="E20" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="F20" s="0" t="s">
-        <v>35</v>
-      </c>
       <c r="G20" s="2" t="s">
         <v>10</v>
       </c>
@@ -6120,7 +9768,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>385</v>
@@ -6128,8 +9776,8 @@
       <c r="C21" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="E21" s="0" t="s">
-        <v>47</v>
+      <c r="F21" s="0" t="s">
+        <v>9</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>10</v>
@@ -6137,36 +9785,7 @@
       <c r="H21" s="0" t="n">
         <v>9805674556</v>
       </c>
-      <c r="I21" s="0" t="s">
-        <v>11</v>
-      </c>
       <c r="J21" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="s">
-        <v>410</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H22" s="0" t="n">
-        <v>9805674556</v>
-      </c>
-      <c r="J22" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -6175,9 +9794,9 @@
     <hyperlink ref="G2" r:id="rId1" display="mamta.mehta@algoworks.com"/>
     <hyperlink ref="G3" r:id="rId2" display="mamta.mehta@algoworks.com"/>
     <hyperlink ref="G4" r:id="rId3" display="mamta.mehta@algoworks.com"/>
-    <hyperlink ref="G6" r:id="rId4" display="mamta.mehta@algoworks.com"/>
-    <hyperlink ref="G9" r:id="rId5" display="mamtamehta@gmail"/>
-    <hyperlink ref="G13" r:id="rId6" display="mamtamehta@gmailcom"/>
+    <hyperlink ref="G8" r:id="rId4" display="mamtamehta@gmail"/>
+    <hyperlink ref="G12" r:id="rId5" display="mamtamehta@gmailcom"/>
+    <hyperlink ref="G13" r:id="rId6" display="mamta.mehta@algoworks.com"/>
     <hyperlink ref="G14" r:id="rId7" display="mamta.mehta@algoworks.com"/>
     <hyperlink ref="G15" r:id="rId8" display="mamta.mehta@algoworks.com"/>
     <hyperlink ref="G16" r:id="rId9" display="mamta.mehta@algoworks.com"/>
@@ -6186,7 +9805,6 @@
     <hyperlink ref="G19" r:id="rId12" display="mamta.mehta@algoworks.com"/>
     <hyperlink ref="G20" r:id="rId13" display="mamta.mehta@algoworks.com"/>
     <hyperlink ref="G21" r:id="rId14" display="mamta.mehta@algoworks.com"/>
-    <hyperlink ref="G22" r:id="rId15" display="mamta.mehta@algoworks.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>